<commit_message>
Submitted to JLCPCB 2020-07-12
</commit_message>
<xml_diff>
--- a/RFUtilityKnife-BOM.xlsx
+++ b/RFUtilityKnife-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="130">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">100 pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C24,C25</t>
+    <t xml:space="preserve">C1,C64,C24,C25,C60</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitors_SMD:C_0805_HandSoldering</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">100 nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C2,C5,C7,C20,C18,C14,C26,C28,C35,C30,C33,C32,C41,C42,C47,C46,C48,C56,C58,C54</t>
+    <t xml:space="preserve">C2,C5,C7,C20,C18,C14,C26,C28,C35,C30,C33,C32,C41,C47,C46,C48,C56,C58,C54,C39,C44</t>
   </si>
   <si>
     <t xml:space="preserve">C49678</t>
@@ -76,16 +76,16 @@
     <t xml:space="preserve">1 pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitors_SMD:C_0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3,C16,C31,C45,C49</t>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3,C16,C31,C45,C49,C65</t>
   </si>
   <si>
     <t xml:space="preserve">C45783</t>
@@ -94,12 +94,30 @@
     <t xml:space="preserve">10 nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C4,C6,C8,C9,C17,C15,C21,C13,C10,C22,C19,C27,C34,C36,C29,C37,C38,C40,C43,C44,C39,C55,C57,C59,C53</t>
+    <t xml:space="preserve">C4,C6,C8,C9,C17,C15,C21,C10,C19,C13,C23,C27,C34,C36,C29,C40,C43,C55,C57,C59,C53,C37,C42,C38,C66</t>
   </si>
   <si>
     <t xml:space="preserve">C1710</t>
   </si>
   <si>
+    <t xml:space="preserve">15 pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C50,C52,C51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2 uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C61,C62,C63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C49217</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED</t>
   </si>
   <si>
@@ -136,10 +154,28 @@
     <t xml:space="preserve">C95872</t>
   </si>
   <si>
+    <t xml:space="preserve">D_Zener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodes_SMD:D_MiniMELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US1MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C412437</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conn_01x01</t>
   </si>
   <si>
-    <t xml:space="preserve">J1,J5,J14,J15,J8,J9,J6,J10,J16,J17,J12,J13,J7,J11,J100,J101,J98,J99,J130,J131,J128,J129</t>
+    <t xml:space="preserve">J1,J5,J14,J15,J8,J9,J6,J10,J16,J17,J12,J13,J7,J11,J100,J101,J98,J99,J130,J131,J128,J129,J20,J21,J4,J19</t>
   </si>
   <si>
     <t xml:space="preserve">RFUtilityKnife:PadHole</t>
@@ -148,7 +184,7 @@
     <t xml:space="preserve">Barrel_Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">J2</t>
+    <t xml:space="preserve">J2,J22,J23</t>
   </si>
   <si>
     <t xml:space="preserve">Connectors:BARREL_JACK</t>
@@ -157,31 +193,40 @@
     <t xml:space="preserve">Conn_Coaxial</t>
   </si>
   <si>
-    <t xml:space="preserve">J24,J25,J4,J3,J18,J92,J94,J95,J96,J97,J93,J127,J126</t>
+    <t xml:space="preserve">J24,J25,J3,J18,J95,J96,J93,J127,J126</t>
   </si>
   <si>
     <t xml:space="preserve">RFUtilityKnife:Amphenol_RF_SMA_132289</t>
   </si>
   <si>
-    <t xml:space="preserve">J42,J91,J90,J31,J43,J89,J87,J88,J86,J85,J83,J84,J82,J81,J79,J80,J78,J77,J75,J76,J74,J73,J71,J72,J70,J69,J67,J68,J66,J65,J63,J64,J62,J61,J59,J60,J58,J57,J55,J56,J54,J53,J51,J52,J50,J49,J47,J48,J46,J45,J44,J41,J39,J40,J38,J37,J35,J36,J34,J33,J32,J30,J29,J27,J28,J26,J19,J22,J23,J21,J20,J111,J113,J112,J110,J108,J109,J106,J107,J104,J105,J102,J103,J123,J125,J124,J122,J120,J121,J118,J119,J116,J117,J114,J115</t>
+    <t xml:space="preserve">J71,J72,J70,J65,J63,J59,J60,J53,J49,J48,J45,J44,J29,J27,J28,J26,J33,J31,J32,J30</t>
   </si>
   <si>
     <t xml:space="preserve">RFUtilityKnife:BigSlot</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumper_NO_Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP4,JP3,JP2,JP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x02_Pitch2.54mm</t>
+    <t xml:space="preserve">Jumper_NC_Dual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x03_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 uH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductors_SMD:L_7.3x7.3_H4.5</t>
   </si>
   <si>
     <t xml:space="preserve">2SC3356</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1,Q2,Q3,Q8,Q4,Q7,Q6,Q5,Q9,Q10,Q12,Q11,Q13,Q14,Q15,Q16,Q18,Q19,Q21,Q17,Q20,Q22,Q23,Q27,Q28,Q26</t>
+    <t xml:space="preserve">Q1,Q2,Q3,Q7,Q6,Q5,Q4,Q9,Q10,Q12,Q11,Q13,Q14,Q15,Q16,Q18,Q19,Q17,Q23,Q27,Q28,Q26</t>
   </si>
   <si>
     <t xml:space="preserve">TO_SOT_Packages_SMD:SOT-23</t>
@@ -190,10 +235,19 @@
     <t xml:space="preserve">C9659</t>
   </si>
   <si>
+    <t xml:space="preserve">MMBT5551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q25,Q24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2145</t>
+  </si>
+  <si>
     <t xml:space="preserve">1k</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R30,R32,R19,R47,R88,R91</t>
+    <t xml:space="preserve">R1,R30,R47,R88,R91,R93,R95,R97</t>
   </si>
   <si>
     <t xml:space="preserve">Resistors_SMD:R_0805_HandSoldering</t>
@@ -205,112 +259,94 @@
     <t xml:space="preserve">NC</t>
   </si>
   <si>
-    <t xml:space="preserve">R15,R18,R25,R36,R39,R66,R68,R110,R112,R89</t>
+    <t xml:space="preserve">R15,R18,R25,R36,R39,R66,R68,R110,R112</t>
   </si>
   <si>
     <t xml:space="preserve">100k</t>
   </si>
   <si>
-    <t xml:space="preserve">R16</t>
+    <t xml:space="preserve">R16,R89</t>
   </si>
   <si>
     <t xml:space="preserve">C17407</t>
   </si>
   <si>
-    <t xml:space="preserve">0R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R17,R38,R67,R111,R90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17477</t>
+    <t xml:space="preserve">47R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17,R38,R67,R86,R111,R37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3,R11,R33,R21,R45,R63,R46,R107,R98,R96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4,R7,R12,R34,R27,R23,R48,R60,R64,R53,R50,R55,R77,R103,R108,R99,R72,R82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17415</t>
   </si>
   <si>
     <t xml:space="preserve">2k2</t>
   </si>
   <si>
-    <t xml:space="preserve">R20</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C17520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3,R11,R33,R45,R63,R46,R107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17713</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistors_SMD:R_0603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4,R7,R12,R34,R27,R23,R48,R60,R64,R53,R50,R55,R77,R84,R103,R108,R99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17415</t>
+    <t xml:space="preserve">R42,R78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5,R13,R35,R24,R49,R65,R51,R54,R109,R101,R40,R70,R75,R83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6,R14,R26,R52,R61,R71,R102,R81,R94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R69,R41,R79,R76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4310</t>
   </si>
   <si>
     <t xml:space="preserve">100R</t>
   </si>
   <si>
-    <t xml:space="preserve">R40,R42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C22775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C27592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5,R13,R35,R49,R65,R51,R54,R81,R109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6,R14,R26,R21,R52,R61,R79,R83,R71,R72,R69,R70,R102,R98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17414</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R74,R75,R76,R86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C17714</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8,R28,R22,R56,R59,R78,R85,R73,R87,R104,R100</t>
+    <t xml:space="preserve">R8,R20,R28,R56,R59,R73,R104</t>
   </si>
   <si>
     <t xml:space="preserve">C17408</t>
@@ -319,18 +355,30 @@
     <t xml:space="preserve">22R</t>
   </si>
   <si>
-    <t xml:space="preserve">R9,R2,R10,R29,R24,R31,R57,R58,R43,R44,R62,R80,R82,R105,R106,R101</t>
+    <t xml:space="preserve">R9,R2,R10,R29,R22,R31,R57,R58,R43,R44,R62,R80,R105,R106,R90,R74</t>
   </si>
   <si>
     <t xml:space="preserve">C17561</t>
   </si>
   <si>
-    <t xml:space="preserve">RV1,RV2,RV3</t>
+    <t xml:space="preserve">56R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R92,R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1</t>
   </si>
   <si>
     <t xml:space="preserve">Potentiometers:Potentiometer_Triwood_RM-065</t>
   </si>
   <si>
+    <t xml:space="preserve">RV3</t>
+  </si>
+  <si>
     <t xml:space="preserve">LM317MDT</t>
   </si>
   <si>
@@ -341,6 +389,27 @@
   </si>
   <si>
     <t xml:space="preserve">C75510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NE555</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housings_SOIC:SOIC-8_3.9x4.9mm_Pitch1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM78M05_TO252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C58069</t>
   </si>
 </sst>
 </file>
@@ -436,17 +505,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.6"/>
   </cols>
   <sheetData>
@@ -528,13 +597,16 @@
         <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>21</v>
       </c>
@@ -567,59 +639,65 @@
         <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -636,37 +714,37 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="0" t="s">
         <v>55</v>
       </c>
     </row>
@@ -680,58 +758,49 @@
       <c r="C18" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>70</v>
@@ -745,7 +814,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>73</v>
@@ -773,91 +842,88 @@
         <v>79</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="C26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>97</v>
@@ -871,7 +937,7 @@
         <v>99</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>100</v>
@@ -879,27 +945,136 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>102</v>
+        <v>76</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>